<commit_message>
'update scraper for jumia website'
</commit_message>
<xml_diff>
--- a/webscraping/jumia_products.xlsx
+++ b/webscraping/jumia_products.xlsx
@@ -453,680 +453,680 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OPPO A5 Dual SIM 4G 256GB/8GB - Aurora Green</t>
+          <t>Asus Vivobook Go 15 OLED E1504FA-NJ005W( AMD Ryzen5-7520U-8GB LPDDR5-5200Mhz, 512GB M.2 NVMe-AMD Radeon Graphics-15.6-inch FHD 60Hz- Win 11-Cool Silver )</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EGP 9,499.00</t>
+          <t>EGP 18,666.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=OP872MP1WV3K1NAFAMZ-215229284&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL22S3P1NAFAMZ-190092247&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OPPO A5X Dual SIM, 128GB, 4GB RAM, 4G LTE - Laser White</t>
+          <t>Acer  Aspire 3 A315-44P-R4GH AMD Ryzen 7 5700U 512GB SSD 8GB Ram AMD Radeon Graphics 15.6Inch FHD - Silver - NX.KSJEM.004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EGP 7,589.00</t>
+          <t>EGP 17,699.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=OP872MP3ADL2TNAFAMZ-214855777&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AC008CL2SSAJLNAFAMZ-214909254&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Infinix XPAD 20 11.0" Inch Single SIM 4G 128GB/6GB - Stellar Grey</t>
+          <t>HP Renewed ProBook 640 G8 Intel Core i5-1145G7- RAM 16GB - Storage SSD 256GB - GPU Intel Iris Xe Graphics - Grade A+ – Windows – Display 14 INCH FHD - English Keyboard</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EGP 7,255.00</t>
+          <t>EGP 15,499.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/infinix-xpad-20-11.0-inch-single-sim-4g-128gb6gb-stellar-grey-133689175.html</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2U4UGLNAFAMZ-215409438&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Honor 400 Lite Dual SIM 5G 256GB/8GB - Velvet Grey</t>
+          <t>DELL Renewed Latitude 3310 Core i3-8145U - RAM 8GB - Hard SSD 256GB - Display 13.3 INCH - Black - Grade B+ - Windows - English Keyboard</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EGP 12,299.00</t>
+          <t>EGP 7,999.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP2JOCZLNAFAMZ-214910045&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL2ZZ3TTNAFAMZ-215259863&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Honor X5c Plus Dual SIM 4G 128GB/4GB - Midnight Black</t>
+          <t>DELL Preowned Latitude 5300 – i5-8265U Processor - Ram 8 GB DDR4 - Hard 256 GB SSD - VGA Intel UHD Graphics for 8th Generation Intel - Display 13.3'' Inch Led Full HD Screen- Windows 10 Pro  - Grade B - Windows</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EGP 4,725.00</t>
+          <t>EGP 10,000.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP26BRG1NAFAMZ-215287201&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL2U8YJ5NAFAMZ-215284995&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A26 Dual SIM 5G 256GB/8GB Mobile Phone - Black</t>
+          <t>Microsoft Surface Pro 5,intel Core i5 7th GEN (U), 12.3" inch , 8GB Ram - 256GB SSD M.2- Intel® HD Graphics 620</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EGP 13,599.00</t>
+          <t>EGP 13,800.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2CPL71NAFAMZ-212672671&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=MI353CL2N5BODNAFAMZ-215322731&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A26 Dual SIM 5G 256GB/8GB Mobile Phone- Black</t>
+          <t>Asus ASUS Vivobook Go 15 E1504GA-NJ043W- Intel I3 N305 - 4GB - 256GB SSD - 15.6 Inch - Windows 11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EGP 13,599.00</t>
+          <t>EGP 16,299.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2BIXSLNAFAMZ-215056379&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL2RU54ZNAFAMZ-213561832&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi 15C Dual SIM, 256GB, 8GB RAM, 4G LTE - Mint Green</t>
+          <t>Lenovo Yoga L380 X360 , Intel Core i5 8th GEN (U) , 13.3" inch , RAM 8GB , 256GB SSD, Integrated Intel UHD Graphics 620, Windows 11 Pro - Black</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EGP 7,099.00</t>
+          <t>EGP 14,500.00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP1Z4Z0DNAFAMZ-215105760&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL2UQD5HNAFAMZ-215316134&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Honor 400 Lite Dual SIM 5G 256GB/8GB - Velvet Black</t>
+          <t>Acer Aspire 5 A515-57-55KJ Slim Business Laptop NX.KN4EM.008</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EGP 11,999.00</t>
+          <t>EGP 21,499.00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP2DQ0XTNAFAMZ-214910044&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AC008CL24ALE7NAFAMZ-211160037&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A56 – Mobile Phone – 12GB RAM – 256GB – 5G – Awesome Graphite</t>
+          <t>HP Elite Book 855 G7, AMD Ryzen 5 Pro 4650U, 15.6" Inch 16GB Ram, 256GB SSD, AMD Radeon Vega Graphics, Windows 11 - Silver</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EGP 22,999.00</t>
+          <t>EGP 19,000.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2YAYXFNAFAMZ-213301734&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2WBW51NAFAMZ-215378673&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi Note 14 Mobile Phone -6.7 Inches - 256GB/8GB - Dual SIM 4G -Midnight Black</t>
+          <t>Lenovo IdeaPad Slim 3 15AMN8 Laptop AMD Ryzen™ 5 7520U, 8GB, 512GB SSD, AMD Radeon™ 610M, 15.6" FHD, 82XQ00F8ED -</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EGP 9,599.00</t>
+          <t>EGP 21,959.00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP2AFPABNAFAMZ-213302709&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL32FH83NAFAMZ-214204956&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi Note 14 - Dual SIM 4G 256GB/8GB Mobile Phone - Midnight Black</t>
+          <t>DELL Renewed Precision 3560 Mobile Workstation Intel Core i7-1165G7 - RAM 16GB - Hard SSD 512GB - GPU Nvidia Quadro T500 2GB DDR6 Graphics - Grade A - Windows - Display 15.6 Inch FHD - English Keyboard</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EGP 10,129.00</t>
+          <t>EGP 23,999.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP2SRWSBNAFAMZ-212003096&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL2FRWW5NAFAMZ-215436925&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A17 - 6.7" 128GB/6GB Dual SIM 4G Mobile Phone - Black</t>
+          <t>HP Preowned EliteBook 845 G7 Full HD 14Inch AMD Ryzen5 16GB RAM 256GBSSD - Grade B - Windows</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EGP 8,299.00</t>
+          <t>EGP 12,999.00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2D3Z19NAFAMZ-215069618&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2GL3QPNAFAMZ-215175037&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>OPPO A5 Dual SIM 4G 256GB/8GB - Mist White</t>
+          <t>HP Renewed  PROBOOK 435 G8 CPU: AMD RYZEN 3 5400U - RAM: 8GB DDR4 - Storage: 256GB-SSD - GPU: AMD RADEON - DISPLAY: 13.3 INCH TOUCHSCREEN X360 - Silver - Grade A - Windows</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>EGP 9,499.00</t>
+          <t>EGP 13,499.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=OP872MP1QWRI9NAFAMZ-215229283&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2AWR9DNAFAMZ-215259838&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>OPPO Reno 14f Dual SIM 5G 256GB/12GB - Luminous Green</t>
+          <t>Lenovo IdeaPad 5 2 in 1 Laptop Intel® Core i7-13620H, 16GB Ram, 512GB SSD, UHD Graphics, 14" WUXGA, Win 11,83KX0045ED - Luna Grey</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EGP 18,699.00</t>
+          <t>EGP 42,049.00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=OP872MP2EQ3PDNAFAMZ-215229287&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL2N2911NAFAMZ-214860846&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi A5 Dual SIM, 128GB, 4GB RAM, 4G LTE - Midnight Black</t>
+          <t>Asus ASUS Vivobook Go 15 E1504FA-NJ003W -  AMD Ryzen™ 3 7320U Processor 2.8GHz - 4GB - 256 SSD - 15.6 Inch - Windows 11</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EGP 5,079.00</t>
+          <t>EGP 15,816.00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP1WJNR1NAFAMZ-214342971&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL2XSH6RNAFAMZ-213561833&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Honor X5c Plus Dual SIM 4G 128GB/4GB - Ocean Cyan</t>
+          <t>Lenovo  LOQ essential 15IAX9E 83LK0076AD Intel Core i5-12450HX - NVIDIA RTX 2050 4GB - 16GB DDR5 4800MHz - 512GB SSD M.2 - 15.6" FHD IPS 144Hz 100% sRGB - Free Dos - Luna Grey</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EGP 4,725.00</t>
+          <t>EGP 28,888.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP2CA3HTNAFAMZ-215287202&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL36H9OTNAFAMZ-215338246&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A26 Dual SIM 5G 256GB/8GB 6.7 inches Mobile phone - Peach Pink</t>
+          <t>DELL DELL Latitude 5490 CORE I5 8350U</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EGP 13,799.00</t>
+          <t>EGP 11,300.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/samsung-galaxy-a26-dual-sim-5g-256gb8gb-6.7-inches-mobile-phone-peach-pink-133718324.html</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL30KX61NAFAMZ-214954003&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Infinix Note 50S 5G 256/ 8GB Mobile Phone Titaanium Gray with Charger</t>
+          <t>Asus F16 FX607VU-RL805W Gaming Laptop Intel Core 5 210H 512GB SSD 8GB Ram Nvidia GeForce RTX 4050 6GB 16 inch'' FHD+ Win.11 - Mecha Gray</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EGP 12,199.00</t>
+          <t>EGP 42,999.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=IN234MP23OQX5NAFAMZ-215237802&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL2CLNXHNAFAMZ-214864134&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Honor X7d Dual SIM 4G 256GB/8GB - Desert Gold</t>
+          <t>Lenovo Laptop  I7-13620H - 16G - 512Ssd - Uhd-15.6" Fhd - Grey- 83Em007Ved Slim 3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>EGP 8,299.00</t>
+          <t>EGP 34,519.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP34HIZ1NAFAMZ-215090305&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL1YG99RNAFAMZ-188598835&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A17 - 6.7" 128GB/6GB Dual SIM 4G Mobile Phone - Light Blue</t>
+          <t>DELL Renewed Latitude 3310 Core i5-8265U - RAM 8GB - Hard SSD 256GB - GPU Intel UHD Graphics - Grade B - Windows - Display 13.3 INCH HD - English Keyboard</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EGP 8,099.00</t>
+          <t>EGP 9,499.00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2Z2V99NAFAMZ-215069591&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL2B1NYHNAFAMZ-215245837&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi 15C Dual SIM, 256GB, 8GB RAM, 4G LTE - Moonlight Blue</t>
+          <t>HP Renewed ZBook Firefly 14 G8 Intel Core i5-1145G7 - RAM 16GB - Storage SSD 256GB - GPU Intel UHD Grade A - Windows – Display 14 INCH FHD - English Keyboard</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>EGP 7,099.00</t>
+          <t>EGP 16,999.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP1WIVNXNAFAMZ-215106499&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2JM9LPNAFAMZ-215369964&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Honor X5c Dual SIM 4G 64GB/4GB - Midnight Black</t>
+          <t>HP Renewed EliteBook 840 G8 Intel Core i7-1165G7 - RAM 16GB - Storage SSD 512GB - GPU Intel Iris Xe Graphics - Grade A+ – Windows – Display 14 INCH FHD - English Keyboard</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>EGP 3,999.00</t>
+          <t>EGP 18,999.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP2I8FJLNAFAMZ-215287203&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL2C9UB9NAFAMZ-215409435&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>XIAOMI POCO C85 Dual SIM 256/8  Mobile phone - Black + free Mi Wired In-Ear Earphones Basic - Black</t>
+          <t>MSI 15 F13MG CPU Raptor Lake I5-1335U RAM Onboard DDR4 8GB ( 3200MHz ) HDD 512 GB NVMe PCIe SSD UHD Intel Iris Xe Graphics Single Backlight KB (White) 14 FHD (1920*1080) 60Hz IPS – Level(9S7-15S122-057 )</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>EGP 6,990.00</t>
+          <t>EGP 21,999.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP1UMHJTNAFAMZ-215203198&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=MS198CL1S41IBNAFAMZ-210991939&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Honor 400 Lite Dual SIM 5G 256GB/8GB - Marrs Green</t>
+          <t>HP Elite Book 840 G8, Intel Core i7 11th Gen (U), 14" Inch, 16GB Ram, 512GB SSD, Integrated Intel Iris Xe Graphics, Widnows 11 Pro - Silver + Free Bag</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>EGP 12,299.00</t>
+          <t>EGP 30,000.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP2PMP1DNAFAMZ-214910046&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL34X6BLNAFAMZ-215229331&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A26 Dual SIM 5G 256GB/8GB Mobile Phone – Peach Pink</t>
+          <t>DELL Latitude 5500 , Intel Core i7 8th Gen (U), 15.6" Inch, 8GB Ram, 256GB SSD, Integrated Intel UHD Graphics 620, Windows 11 Pro - Black</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>EGP 13,499.00</t>
+          <t>EGP 15,000.00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2OM9ALNAFAMZ-212672673&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL3ABGX5NAFAMZ-215298077&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A56 256GB، 8GB RAM Mobile Phone – 6.7"، 5G, Awesome pink</t>
+          <t>Asus VivoBook 15 Laptop, Intel Core i3-1315U, 8GB Ram, 256GB SSD, Intel UHD, 15.6" Full HD, Win 11, X1504VA-NJ083W - Cool Silver</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>EGP 21,999.00</t>
+          <t>EGP 17,259.00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP1T0YXVNAFAMZ-213473324&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL2NNBTPNAFAMZ-215335442&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A56 Dual SIM 5G 256GB/8GB Mobile Phone - Awesome Light Grey</t>
+          <t>DELL Preowned Latitude 5490 – Intel Core i5-8350U – 8GB Ram – 256GB SSD – Intel UHD Graphics 620 – 14 Inch - Grade B - Windows</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>EGP 20,799.00</t>
+          <t>EGP 10,150.00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP34I7L5NAFAMZ-214983443&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL1U0RWXNAFAMZ-215175054&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi A3x Dual SIM 4G 128GB/4GB Mobile Phone - Midnight Black</t>
+          <t>TAGITOP Flip-Intel Core i5 8th Generation8259U-8 GB DDR4 RAM-256 GB SSD-Touch Panel 14.1” FHD-Intel Iris Plus Graphics 655</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>EGP 4,509.00</t>
+          <t>EGP 26,000.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP2AA3QRNAFAMZ-214211987&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=TA628CL023XHQNAFAMZ-97473238&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Honor 400 Dual SIM 5G Smartphone - 512GB/12GB - Midnight Black</t>
+          <t>HP Zbook 15 G6, Intel i7 9th Gen (H), 15.6" Inch, 32GB Ram, 512GB SSD, Integrated NVIDIA Quadro T2000 GDDR5 (4GB), Windows 10 - Dark Grey</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>EGP 22,999.00</t>
+          <t>EGP 30,000.00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP1NO57DNAFAMZ-215204658&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL37XN6LNAFAMZ-214806570&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Itel A50c Dual SIM 4G 64GB/2GB - Dawn Blue</t>
+          <t>DELL Renewed Latitude 7420 – Core i7-1185G7 – Intel Iris Xe Graphics – 32GB RAM – 512GB SSD – gray - Grade B</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>EGP 2,799.00</t>
+          <t>EGP 20,500.00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=IT359MP21WG3TNAFAMZ-215237772&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL38QCFTNAFAMZ-214951590&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Honor 400 Pro Dual SIM 5G Smartphone - 512GB/12GB - Lunar Grey</t>
+          <t>DELL Renewed Latitude 3490 Intel Core I5-8250U - RAM 8GB - Storage SSD 256GB -  GPU Intel UHD Graphics - Grade B+ - Windows – Display 14 INCH HD – English Keyboard</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>EGP 32,499.00</t>
+          <t>EGP 9,999.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP1QTI59NAFAMZ-215060072&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL31DIPXNAFAMZ-215434601&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Itel A50c Dual SIM 4G 64GB/2GB  - Sapphire  Black</t>
+          <t>Lenovo Loq 15IAX9 Laptop, Intel® Core i5-12450HX, 12GB Ram, 512GB SSD, NVIDIA® GeForce RTX™ 2050 4GB, 15.6" FHD, 83GS00SKED - Luna Grey</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>EGP 3,444.00</t>
+          <t>EGP 33,259.00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=IT359MP1VY421NAFAMZ-215237771&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL2WSORPNAFAMZ-214851493&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>OPPO Reno 14f Dual SIM 5G 256GB/12GB - Opal Blue</t>
+          <t>Foldable Laptop Table And Bed</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>EGP 19,015.00</t>
+          <t>EGP 275.00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=OP872MP2RXH1XNAFAMZ-215080177&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=GE810FD2TY2VENAFAMZ-202862598&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A07 Dual SIM, 128GB, 4GB RAM, 4G LTE - Black</t>
+          <t>HP Zbook 15 G5, Intel i7 8th Gen (H), 15.6" Inch, 32GB Ram, 512GB SSD, NVIDIA Quadro P1000 GDDR5 (4GB), Windows 10 Pro - Dark Gray</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>EGP 5,969.00</t>
+          <t>EGP 25,999.00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP20PH1DNAFAMZ-215165113&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HP431CL27IWGDNAFAMZ-214763693&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>XIAOMI Redmi 15C Dual SIM, 128GB, 6GB RAM, 4G LTE - Midnight Black</t>
+          <t>DELL Renewed Latitude 7420 – Core i7-1185G7 – Intel Iris Xe Graphics – 32GB RAM – 512GB SSD – gray - Grade B - Windows</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>EGP 6,289.00</t>
+          <t>EGP 20,200.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=XI606MP2IKZMLNAFAMZ-215090718&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL34ZVJLNAFAMZ-215175051&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A07 Dual SIM, 64GB, 4GB RAM, 4G LTE - Black</t>
+          <t>DELL Latitude 5400 , Intel Core i7 8th Gen (U), 14" Inch, 8GB Ram, 256GB SSD, Integrated Intel UHD Graphics 620, Windows 11 Pro - Black</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>EGP 5,069.00</t>
+          <t>EGP 12,500.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2OKYE9NAFAMZ-215165435&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=DE014CL2R9LK9NAFAMZ-215298044&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A07 4GB-64GB Mobile Phone Dual SIM 4G - Black</t>
+          <t>Lenovo Loq Laptop Intel Core i7-14700HX, 24GB Ram, 512GB SSD, NVIDIA® GeForce RTX™ 5050 8GB, 15.6" FHD, 83JE00DBED - Luna Grey</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>EGP 5,060.00</t>
+          <t>EGP 62,649.00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2QZ2MLNAFAMZ-215144854&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL324AX1NAFAMZ-214859628&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A06 - 6.7-inch 6GB/128GB Dual Sim 4G - Mobile Phone - Black</t>
+          <t>Lenovo IdeaPad Slim 3, Intel® Core i5-13420H, 8GB Ram, 512GB SSD, UHD, 15.6" FHD, 83EM00KGED - Arctic Grey</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>EGP 6,089.00</t>
+          <t>EGP 25,939.00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=SA024MP2KD0P3NAFAMZ-211121698&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=LE018CL333PRHNAFAMZ-215034737&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Honor X6c Dual SIM, 128GB, 6GB RAM, 4G LTE - Moonlight White</t>
+          <t>Asus Laptop I7 -1355U - 8G - 512 Ssd - Uhd -15.6 Fhd - Win11 - Quiet Blue-X1504Va-Nj017W</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>EGP 5,909.00</t>
+          <t>EGP 28,769.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=HO474MP37EECXNAFAMZ-214990016&amp;return=%2Fcatalog%2F%3Fq%3Dphone</t>
+          <t>https://www.jumia.com.eg/customer/account/login/?tkWl=AS040CL1T423QNAFAMZ-183433408&amp;return=%2Fcatalog%2F%3Fq%3Dlaptop</t>
         </is>
       </c>
     </row>

</xml_diff>